<commit_message>
Edited BOM and setting coding folder
</commit_message>
<xml_diff>
--- a/Darby Stuff/BOM 3_3_2020.xlsx
+++ b/Darby Stuff/BOM 3_3_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\GitHub\TNCMCU\Darby Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D48E0-9608-4C06-8354-BAF68AE8827D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DEF2E5-F459-452F-88A3-FFE404FA8126}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="24516" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19872" yWindow="864" windowWidth="24516" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>Purchase Link</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/15033</t>
-  </si>
-  <si>
-    <t>USB Logic Analyzer - 25MHz/8-Channel</t>
-  </si>
-  <si>
     <t>3PCS 400 tie-Points breadboard</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>https://store.digilentinc.com/analog-discovery-2-100msps-usb-oscilloscope-logic-analyzer-and-variable-power-supply/</t>
+  </si>
+  <si>
+    <t>Analog Discovery 2</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -501,10 +501,10 @@
     </row>
     <row r="3" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6">
         <v>0.88</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="4" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6">
         <v>7.95</v>
@@ -537,10 +537,10 @@
     </row>
     <row r="5" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6">
         <v>7.95</v>
@@ -555,28 +555,28 @@
     </row>
     <row r="6" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6">
-        <v>19.95</v>
+        <v>279</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>59.849999999999994</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6">
         <v>7.98</v>
@@ -594,17 +594,17 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6">
         <v>0.95</v>
       </c>
       <c r="D8" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>2.8499999999999996</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -612,17 +612,17 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6">
         <v>5.79</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>5.79</v>
+        <v>17.37</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -634,7 +634,7 @@
       </c>
       <c r="E10" s="6">
         <f>SUM(E2:E9)</f>
-        <v>143.16999999999999</v>
+        <v>380.55</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
I've added a lot. I've also tried to add files as HTML that will load the webpage for you
</commit_message>
<xml_diff>
--- a/Darby Stuff/BOM 3_3_2020.xlsx
+++ b/Darby Stuff/BOM 3_3_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\GitHub\TNCMCU\Darby Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DEF2E5-F459-452F-88A3-FFE404FA8126}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F14D65F-D6F5-4269-927C-B2034AD6241A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19872" yWindow="864" windowWidth="24516" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1632" yWindow="3216" windowWidth="24516" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>STM32F446RE Nucleo board</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Analog Discovery 2</t>
+  </si>
+  <si>
+    <t>Kobe</t>
+  </si>
+  <si>
+    <t>Received (by)</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,13 +128,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,11 +158,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,8 +187,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -452,7 +475,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,6 +485,7 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -480,6 +504,9 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -498,6 +525,9 @@
         <f>C2*D2</f>
         <v>42</v>
       </c>
+      <c r="F2" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -516,6 +546,9 @@
         <f t="shared" ref="E3:E9" si="0">C3*D3</f>
         <v>8.8000000000000007</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -534,6 +567,9 @@
         <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
+      <c r="F4" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -552,6 +588,9 @@
         <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -570,6 +609,9 @@
         <f t="shared" si="0"/>
         <v>279</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -588,6 +630,9 @@
         <f t="shared" si="0"/>
         <v>7.98</v>
       </c>
+      <c r="F7" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -606,6 +651,9 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
+      <c r="F8" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -623,6 +671,9 @@
       <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>17.37</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>